<commit_message>
Read testcase names and data from excel to drive the test.
</commit_message>
<xml_diff>
--- a/test_data/TestCaseNames.xlsx
+++ b/test_data/TestCaseNames.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,39 +11,33 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
-  <si>
-    <t>UserName_test_1</t>
-  </si>
-  <si>
-    <t>TC#</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>ExecutinFlag</t>
-  </si>
-  <si>
-    <t>Password_test_2</t>
-  </si>
-  <si>
-    <t>Validate_login_complete_test_3</t>
   </si>
   <si>
     <t>Y</t>
   </si>
   <si>
-    <t>N</t>
+    <t>001_GoodSignin</t>
+  </si>
+  <si>
+    <t>002_BadSignin</t>
+  </si>
+  <si>
+    <t>TC_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,7 +157,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -198,7 +191,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -374,49 +366,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -425,24 +409,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>